<commit_message>
Cleaned up for first sharing
</commit_message>
<xml_diff>
--- a/examples/services.xlsx
+++ b/examples/services.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t xml:space="preserve">Category</t>
   </si>
@@ -47,6 +47,27 @@
   </si>
   <si>
     <t xml:space="preserve">1.1.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Book</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.0.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JSON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GetPassengerList</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.4.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GetFlightList</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.3.4</t>
   </si>
 </sst>
 </file>
@@ -61,6 +82,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -142,10 +164,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -206,6 +228,57 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>